<commit_message>
ADD openai api support
</commit_message>
<xml_diff>
--- a/xlsx/Final.xlsx
+++ b/xlsx/Final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,15 +476,19 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Son movidas, gana massa baja el dólar para que su campaña sea excelente</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2023-10-09 17:51:51</t>
+          <t>10-10-2023</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>liberalesargentinaok</t>
+          <t>franquiito.02</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -494,7 +498,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>tristeza</t>
+          <t>alegría</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -516,17 +520,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Son movidas, gana massa baja el dólar para que su campaña sea excelente</t>
+          <t>100% dee acuerdo</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-10-10 12:56:51</t>
+          <t>09-10-2023</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>franquiito.02</t>
+          <t>fernando_taboas</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -563,7 +567,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-10-10 10:22:27</t>
+          <t>10-10-2023</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -606,7 +610,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2023-10-10 15:27:40</t>
+          <t>10-10-2023</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -648,7 +652,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2023-10-10 17:22:52</t>
+          <t>10-10-2023</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -685,17 +689,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>100% dee acuerdo</t>
+          <t>1050, antes de que gane Alberto yo me agarraba de los pelos, era obvio lo que iba a pasar pero los K tiraron de la soga y ya se está por romperrr</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023-10-09 20:32:34</t>
+          <t>10-10-2023</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>fernando_taboas</t>
+          <t>martin_zingoni</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -705,7 +709,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>alegría</t>
+          <t>sorpresa</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -732,7 +736,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2023-10-10 17:28:07</t>
+          <t>10-10-2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -769,17 +773,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1050, antes de que gane Alberto yo me agarraba de los pelos, era obvio lo que iba a pasar pero los K tiraron de la soga y ya se está por romperrr</t>
+          <t>#MassaPresidente</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2023-10-10 12:57:44</t>
+          <t>09-10-2023</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>martin_zingoni</t>
+          <t>drgustavovaldez</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -789,7 +793,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>sorpresa</t>
+          <t>alegría</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -811,17 +815,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>#MassaPresidente</t>
+          <t>Un desastre</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2023-10-09 22:42:02</t>
+          <t>10-10-2023</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>drgustavovaldez</t>
+          <t>silvina.harris</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -858,7 +862,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2023-10-10 17:48:10</t>
+          <t>10-10-2023</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -895,17 +899,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Un desastre</t>
+          <t>Ustedes dan vergüenza</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2023-10-10 03:46:35</t>
+          <t>10-10-2023</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>silvina.harris</t>
+          <t>zarpadomal1959</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -915,7 +919,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>alegría</t>
+          <t>asco</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -937,27 +941,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Ustedes dan vergüenza</t>
+          <t>Si quieren terminar con el Kirchnerismo, Juntos por el Cambio debe apoyar a Javier Milei y el 19 de Noviembre terminan arrasando. Es simple. No jodan.</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2023-10-10 10:05:33</t>
+          <t>23-10-2023</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>zarpadomal1959</t>
+          <t>lanatappt</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.threads.net/@liberalesargentinaok/post/CyMS-ONuuaU</t>
+          <t>https://www.threads.net/@lanatappt/post/CyvjalRg-vx</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>asco</t>
+          <t>enojo</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -979,17 +983,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Si quieren terminar con el Kirchnerismo, Juntos por el Cambio debe apoyar a Javier Milei y el 19 de Noviembre terminan arrasando. Es simple. No jodan.</t>
+          <t>La anti ética dixit...🤦‍♀️</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2023-10-23 10:28:57</t>
+          <t>26-10-2023</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>lanatappt</t>
+          <t>veronicacepedaph</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -999,7 +1003,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>enojo</t>
+          <t>sorpresa</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1021,17 +1025,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>La anti ética dixit...🤦‍♀️</t>
+          <t>Te acordás cuándo estabas al frente de revista veintitrés? Te cabía Chávez, fidel y le dabas chirlos a Macri mientras fumabas en la ducha?</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2023-10-26 01:29:22</t>
+          <t>24-10-2023</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>veronicacepedaph</t>
+          <t>leover.ok</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1041,7 +1045,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>sorpresa</t>
+          <t>alegría</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1063,17 +1067,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Te acordás cuándo estabas al frente de revista veintitrés? Te cabía Chávez, fidel y le dabas chirlos a Macri mientras fumabas en la ducha?</t>
+          <t>No hay otra posibilidad sino Ezeiza</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2023-10-24 04:48:22</t>
+          <t>25-10-2023</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>leover.ok</t>
+          <t>mariasusana_sartori</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1083,7 +1087,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>alegría</t>
+          <t>sorpresa</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1105,17 +1109,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>No hay otra posibilidad sino Ezeiza</t>
+          <t>Que Antipatria y Facho que sos Lanata, remítete a decir tu opinión ,No a decirle a la gente lo que tiene que hacer.</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2023-10-25 22:55:09</t>
+          <t>24-10-2023</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>mariasusana_sartori</t>
+          <t>kristellrosario</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1125,7 +1129,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>sorpresa</t>
+          <t>enojo</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1147,17 +1151,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Que Antipatria y Facho que sos Lanata, remítete a decir tu opinión ,No a decirle a la gente lo que tiene que hacer.</t>
+          <t>Mediquese</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2023-10-24 00:48:36</t>
+          <t>24-10-2023</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>kristellrosario</t>
+          <t>_g_a_b_r_i_e_a</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1189,17 +1193,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Mediquese</t>
+          <t>Coherencia y dignidad nunca no?</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2023-10-24 00:00:19</t>
+          <t>25-10-2023</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>_g_a_b_r_i_e_a</t>
+          <t>ivanburaok</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1231,17 +1235,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Ni empedo. Votan todos a masa. Gana por afano.. literal</t>
+          <t>NOAMILEI</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2023-10-23 23:15:53</t>
+          <t>24-10-2023</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>juan.andres.castro</t>
+          <t>florviterbo</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1251,7 +1255,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>enojo</t>
+          <t>alegría</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1265,216 +1269,6 @@
         </is>
       </c>
       <c r="H20" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Por afano sería, por afanar claro! Termos</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>2023-10-24 11:07:40</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>alengraziano2</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>https://www.threads.net/@lanatappt/post/CyvjalRg-vx</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>enojo</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Coherencia y dignidad nunca no?</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>2023-10-25 16:45:20</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>ivanburaok</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>https://www.threads.net/@lanatappt/post/CyvjalRg-vx</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>enojo</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>NOAMILEI</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>2023-10-24 22:45:17</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>florviterbo</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>https://www.threads.net/@lanatappt/post/CyvjalRg-vx</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>alegría</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Es precisamente lo contrario. Si Massa gana tomará el control total del peronismo y correrá definitivamente al kirchnerismo a una posición marginal. Si Massa pierde, el kirchnerismo verá una oportunidad para señalar que el error fue poner a un no kirchnerista y volverá a luchar por el dominio del peronismo, del que hoy ya se encuentra lejos</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>2023-10-24 17:52:51</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>acostaandrada</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>https://www.threads.net/@lanatappt/post/CyvjalRg-vx</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>tristeza</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Si estudias HISTORIA, no defenderías el peronismo. Nadie que se precie de ser humanitario, lo respaldaría. Amigo de Hitler, asilador de alemanes asesinos. Lavó el cerebro a toda una generación. Leé los libros escolares de du época. Informate y dejarás de ser peronista. Gsrantizado.</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>2023-10-25 22:40:35</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>patocorte1216</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>https://www.threads.net/@lanatappt/post/CyvjalRg-vx</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>enojo</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>N/E</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
         <is>
           <t>N/E</t>
         </is>

</xml_diff>